<commit_message>
Update summary (windows) max.xlsx
</commit_message>
<xml_diff>
--- a/ForegroundJobScheduler/results/Nonoverlapping windows/summary (windows) max.xlsx
+++ b/ForegroundJobScheduler/results/Nonoverlapping windows/summary (windows) max.xlsx
@@ -1926,10 +1926,18 @@
       <c r="E69" t="n">
         <v>3000.0</v>
       </c>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
+      <c r="F69" t="n">
+        <v>0.336597177186369</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.982395743682028</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.8672130208034844</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.15955614281464672</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
@@ -2374,10 +2382,18 @@
       <c r="E85" t="n">
         <v>3000.0</v>
       </c>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
+      <c r="F85" t="n">
+        <v>0.5222320615886314</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.9536146576023876</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.8415995410760809</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0.15607133643467624</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">

</xml_diff>